<commit_message>
Defined the network based on distance file
</commit_message>
<xml_diff>
--- a/Data/distances.xlsx
+++ b/Data/distances.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5514800-B871-4478-A07F-4A9631F9D9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{E5514800-B871-4478-A07F-4A9631F9D9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{047DAA64-BB9A-4AC2-81FC-620F4A14E577}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13095" windowHeight="23400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sea" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="35">
   <si>
     <t>Fra</t>
   </si>
@@ -140,17 +140,27 @@
   </si>
   <si>
     <t>We removed Sør-Sverige to Nord-Sverige and Sør-Sverige to Europa. This is in line with the capacities in the capacities file</t>
+  </si>
+  <si>
+    <t>Route</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,25 +219,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -319,23 +384,23 @@
   </dxfs>
   <tableStyles count="4">
     <tableStyle name="Sea-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="12"/>
+      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+    </tableStyle>
+    <tableStyle name="Road-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="10"/>
       <tableStyleElement type="firstRowStripe" dxfId="9"/>
       <tableStyleElement type="secondRowStripe" dxfId="8"/>
     </tableStyle>
-    <tableStyle name="Road-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Rail-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
       <tableStyleElement type="headerRow" dxfId="7"/>
       <tableStyleElement type="firstRowStripe" dxfId="6"/>
       <tableStyleElement type="secondRowStripe" dxfId="5"/>
     </tableStyle>
-    <tableStyle name="Rail-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
-    </tableStyle>
     <tableStyle name="Rail-style 2" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -350,40 +415,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:C13">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:D13">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fra"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Til"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Km - sjø"/>
+    <tableColumn id="4" xr3:uid="{E738C402-C91D-40C6-9769-1A27D894B987}" name="Route" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Sea-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:C23">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:D23">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Fra"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Til"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Km - road"/>
+    <tableColumn id="4" xr3:uid="{A138709B-F628-47E6-ACD2-020D68574D70}" name="Route" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Road-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="A1:C15">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="A1:D15">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Fra"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Til"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Km - rail"/>
+    <tableColumn id="4" xr3:uid="{EBF906D1-AF42-4A41-8A67-EE82962C5635}" name="Route" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Rail-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="K3:M7" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="L3:N7" headerRowCount="0">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2"/>
@@ -591,21 +659,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,12 +683,15 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -630,8 +701,11 @@
       <c r="C2" s="1">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -641,8 +715,11 @@
       <c r="C3" s="1">
         <v>190</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -652,8 +729,11 @@
       <c r="C4" s="1">
         <v>290</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -663,8 +743,11 @@
       <c r="C5" s="1">
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -674,8 +757,11 @@
       <c r="C6" s="1">
         <v>530</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -685,8 +771,11 @@
       <c r="C7" s="1">
         <v>250</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -696,8 +785,11 @@
       <c r="C8" s="1">
         <v>210</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -707,8 +799,11 @@
       <c r="C9" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -718,8 +813,11 @@
       <c r="C10" s="1">
         <v>580</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -729,8 +827,11 @@
       <c r="C11" s="1">
         <v>450</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -740,8 +841,11 @@
       <c r="C12" s="3">
         <v>550</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -751,7 +855,10 @@
       <c r="C13" s="1">
         <v>0</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>30</v>
       </c>
     </row>
@@ -766,21 +873,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C944"/>
+  <dimension ref="A1:D944"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D2" sqref="D2:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,8 +897,11 @@
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -801,8 +911,11 @@
       <c r="C2" s="1">
         <v>463</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -812,8 +925,11 @@
       <c r="C3" s="1">
         <v>132</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -823,8 +939,11 @@
       <c r="C4" s="1">
         <v>126</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -834,8 +953,11 @@
       <c r="C5" s="1">
         <v>527</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -845,8 +967,11 @@
       <c r="C6" s="1">
         <v>814</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -856,8 +981,11 @@
       <c r="C7" s="1">
         <v>210</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -867,8 +995,11 @@
       <c r="C8" s="1">
         <v>400</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -878,8 +1009,11 @@
       <c r="C9" s="1">
         <v>476</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -889,8 +1023,11 @@
       <c r="C10" s="1">
         <v>422</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -900,8 +1037,11 @@
       <c r="C11" s="1">
         <v>381</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -911,8 +1051,11 @@
       <c r="C12" s="1">
         <v>299</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -922,8 +1065,11 @@
       <c r="C13" s="1">
         <v>701</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -933,8 +1079,11 @@
       <c r="C14" s="1">
         <v>776</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -944,8 +1093,11 @@
       <c r="C15" s="1">
         <v>623</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -955,8 +1107,11 @@
       <c r="C16" s="1">
         <v>233</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -966,8 +1121,11 @@
       <c r="C17" s="1">
         <v>179</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -977,8 +1135,11 @@
       <c r="C18" s="1">
         <v>422</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -988,8 +1149,11 @@
       <c r="C19" s="1">
         <v>559</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -999,8 +1163,11 @@
       <c r="C20" s="1">
         <v>533</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1010,8 +1177,11 @@
       <c r="C21" s="1">
         <v>591</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1021,8 +1191,11 @@
       <c r="C22" s="1">
         <v>918</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1032,16 +1205,19 @@
       <c r="C23" s="1">
         <v>637</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1965,23 +2141,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M896"/>
+  <dimension ref="A1:N896"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1992,16 +2168,19 @@
         <v>19</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2011,14 +2190,17 @@
       <c r="C2" s="1">
         <v>126</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2028,12 +2210,15 @@
       <c r="C3" s="1">
         <v>506</v>
       </c>
-      <c r="J3" s="7"/>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2043,15 +2228,18 @@
       <c r="C4" s="3">
         <v>146</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2061,15 +2249,18 @@
       <c r="C5" s="3">
         <v>219</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2079,15 +2270,18 @@
       <c r="C6" s="1">
         <v>805</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="7"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="8"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2097,12 +2291,15 @@
       <c r="C7" s="1">
         <v>233</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="9"/>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="7"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="9"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -2112,12 +2309,15 @@
       <c r="C8" s="1">
         <v>330</v>
       </c>
-      <c r="J8" s="7"/>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2127,15 +2327,18 @@
       <c r="C9" s="1">
         <v>426</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -2145,11 +2348,14 @@
       <c r="C10" s="1">
         <v>436</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -2159,11 +2365,14 @@
       <c r="C11" s="1">
         <v>550</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2173,8 +2382,11 @@
       <c r="C12" s="1">
         <v>729</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -2184,11 +2396,14 @@
       <c r="C13" s="1">
         <v>560</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2198,8 +2413,11 @@
       <c r="C14" s="1">
         <v>375</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2209,11 +2427,14 @@
       <c r="C15" s="1">
         <v>650</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cleaning up spatial info
- removing not used files
- mainly updating the data related to spatial information
</commit_message>
<xml_diff>
--- a/Data/distances.xlsx
+++ b/Data/distances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{E5514800-B871-4478-A07F-4A9631F9D9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC37C14B-1A10-4F8D-8DB9-C5893CACA2E1}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{E5514800-B871-4478-A07F-4A9631F9D9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78EDD951-FC2A-4C0D-ADA4-0D1F72F56400}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sea" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="50">
   <si>
     <t>Fra</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Rail</t>
   </si>
   <si>
-    <t>Distance (km)</t>
-  </si>
-  <si>
     <t>From</t>
   </si>
   <si>
@@ -186,17 +183,30 @@
   </si>
   <si>
     <t>comment SJB: we changed this again. Should be included</t>
+  </si>
+  <si>
+    <t>DistanceKM</t>
+  </si>
+  <si>
+    <t>USE TOGETHER SHEET!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -266,6 +276,14 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -295,26 +313,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,10 +544,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:D14">
   <tableColumns count="4">
@@ -588,7 +597,7 @@
     <tableColumn id="1" xr3:uid="{F3648BE0-72E5-4F5B-B00C-79D612E6FF75}" name="Mode"/>
     <tableColumn id="5" xr3:uid="{C257CCC7-A6DA-4311-BA8A-E1A4299D2C3F}" name="From" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{16FA6ECB-F203-4345-B601-2DDCF157928F}" name="To"/>
-    <tableColumn id="3" xr3:uid="{97B9FAAE-E0F2-4577-BF9E-B2C43DFE1756}" name="Distance (km)"/>
+    <tableColumn id="3" xr3:uid="{97B9FAAE-E0F2-4577-BF9E-B2C43DFE1756}" name="DistanceKM"/>
     <tableColumn id="4" xr3:uid="{6CBE1ABD-35AA-432F-8396-2B094DA916FD}" name="Route" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Sea-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -796,7 +805,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -817,13 +826,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -835,7 +844,7 @@
       <c r="C2" s="1">
         <v>170</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -849,7 +858,7 @@
       <c r="C3" s="1">
         <v>190</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
     </row>
@@ -863,7 +872,7 @@
       <c r="C4" s="1">
         <v>290</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
@@ -877,7 +886,7 @@
       <c r="C5" s="1">
         <v>270</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
     </row>
@@ -891,7 +900,7 @@
       <c r="C6" s="1">
         <v>530</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>
@@ -905,7 +914,7 @@
       <c r="C7" s="1">
         <v>250</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
     </row>
@@ -919,17 +928,17 @@
       <c r="C8" s="1">
         <v>210</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -942,7 +951,7 @@
       <c r="C9" s="1">
         <v>180</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
     </row>
@@ -956,7 +965,7 @@
       <c r="C10" s="1">
         <v>580</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
     </row>
@@ -970,52 +979,55 @@
       <c r="C11" s="1">
         <v>450</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1">
         <v>550</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
       </c>
+      <c r="I13" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14">
         <v>1000</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1033,7 +1045,7 @@
   <dimension ref="A1:H944"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D24"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1054,7 +1066,7 @@
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1068,7 +1080,7 @@
       <c r="C2" s="1">
         <v>463</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1082,7 +1094,7 @@
       <c r="C3" s="1">
         <v>132</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1096,7 +1108,7 @@
       <c r="C4" s="1">
         <v>126</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1110,7 +1122,7 @@
       <c r="C5" s="1">
         <v>527</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1124,17 +1136,17 @@
       <c r="C6" s="1">
         <v>814</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
         <v>42</v>
-      </c>
-      <c r="H6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1147,7 +1159,7 @@
       <c r="C7" s="1">
         <v>210</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1161,7 +1173,7 @@
       <c r="C8" s="1">
         <v>400</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1175,7 +1187,7 @@
       <c r="C9" s="1">
         <v>476</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1189,7 +1201,7 @@
       <c r="C10" s="1">
         <v>422</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1203,7 +1215,7 @@
       <c r="C11" s="1">
         <v>381</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1217,7 +1229,7 @@
       <c r="C12" s="1">
         <v>299</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1231,8 +1243,11 @@
       <c r="C13" s="1">
         <v>701</v>
       </c>
-      <c r="D13" s="2">
-        <v>1</v>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1245,7 +1260,7 @@
       <c r="C14" s="1">
         <v>776</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1259,7 +1274,7 @@
       <c r="C15" s="1">
         <v>623</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1273,7 +1288,7 @@
       <c r="C16" s="1">
         <v>233</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1287,7 +1302,7 @@
       <c r="C17" s="1">
         <v>179</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1301,7 +1316,7 @@
       <c r="C18" s="1">
         <v>422</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1315,7 +1330,7 @@
       <c r="C19" s="1">
         <v>559</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1329,7 +1344,7 @@
       <c r="C20" s="1">
         <v>533</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1343,7 +1358,7 @@
       <c r="C21" s="1">
         <v>591</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1357,7 +1372,7 @@
       <c r="C22" s="1">
         <v>918</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1371,12 +1386,12 @@
       <c r="C23" s="1">
         <v>637</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B24" t="s">
@@ -1385,14 +1400,14 @@
       <c r="C24">
         <v>1118</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="9">
         <v>1</v>
       </c>
       <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" t="s">
         <v>45</v>
-      </c>
-      <c r="H24" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2328,8 +2343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N896"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2343,25 +2358,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2375,15 +2390,15 @@
       <c r="C2" s="1">
         <v>126</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="12" t="s">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2395,57 +2410,57 @@
       <c r="C3" s="1">
         <v>506</v>
       </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>146</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>219</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2457,16 +2472,16 @@
       <c r="C6" s="1">
         <v>805</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="7"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2478,13 +2493,13 @@
       <c r="C7" s="1">
         <v>233</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="7"/>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -2496,13 +2511,13 @@
       <c r="C8" s="1">
         <v>330</v>
       </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2514,16 +2529,16 @@
       <c r="C9" s="1">
         <v>426</v>
       </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -2535,10 +2550,10 @@
       <c r="C10" s="1">
         <v>436</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2552,10 +2567,10 @@
       <c r="C11" s="1">
         <v>550</v>
       </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2569,7 +2584,7 @@
       <c r="C12" s="1">
         <v>729</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2583,11 +2598,14 @@
       <c r="C13" s="1">
         <v>560</v>
       </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2600,7 +2618,7 @@
       <c r="C14" s="1">
         <v>375</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2614,15 +2632,15 @@
       <c r="C15" s="1">
         <v>650</v>
       </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
@@ -2631,62 +2649,62 @@
       <c r="C16">
         <v>1118</v>
       </c>
-      <c r="D16" s="15">
-        <v>1</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>45</v>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C17">
         <v>650</v>
       </c>
-      <c r="D17" s="15">
-        <v>1</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>45</v>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C18">
         <v>1000</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="9">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C19">
         <v>630</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="9">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3580,247 +3598,247 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80CA0C3-2A25-494A-9AB6-49EFDFC8B05A}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>170</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>190</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>290</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>270</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>530</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>250</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>210</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>180</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>580</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>450</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>550</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14">
         <v>1000</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="10">
         <v>1</v>
       </c>
     </row>
@@ -3828,16 +3846,16 @@
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>463</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3845,16 +3863,16 @@
       <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>132</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3862,16 +3880,16 @@
       <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>126</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3879,16 +3897,16 @@
       <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>527</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3896,16 +3914,16 @@
       <c r="A19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>814</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3913,16 +3931,16 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>210</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3930,16 +3948,16 @@
       <c r="A21" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>400</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3947,16 +3965,16 @@
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>476</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3964,16 +3982,16 @@
       <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>422</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3981,16 +3999,16 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>381</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3998,16 +4016,16 @@
       <c r="A25" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>299</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4015,16 +4033,16 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>701</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4032,16 +4050,16 @@
       <c r="A27" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>776</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4049,16 +4067,16 @@
       <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>623</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4066,16 +4084,16 @@
       <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>233</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4083,16 +4101,16 @@
       <c r="A30" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>179</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4100,16 +4118,16 @@
       <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>422</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4117,16 +4135,16 @@
       <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>559</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4134,16 +4152,16 @@
       <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>533</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4151,16 +4169,16 @@
       <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>591</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4168,16 +4186,16 @@
       <c r="A35" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>918</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4185,16 +4203,16 @@
       <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>637</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4202,7 +4220,7 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C37" t="s">
@@ -4211,7 +4229,7 @@
       <c r="D37">
         <v>1118</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="9">
         <v>1</v>
       </c>
     </row>
@@ -4219,16 +4237,16 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="1">
         <v>126</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4236,16 +4254,16 @@
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="1">
         <v>506</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4253,16 +4271,16 @@
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="1">
         <v>146</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4273,13 +4291,13 @@
       <c r="B41" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="1">
         <v>219</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4287,16 +4305,16 @@
       <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <v>805</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4304,16 +4322,16 @@
       <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <v>233</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4321,16 +4339,16 @@
       <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="1">
         <v>330</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4338,16 +4356,16 @@
       <c r="A45" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="1">
         <v>426</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4355,16 +4373,16 @@
       <c r="A46" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="1">
         <v>436</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="1">
         <v>2</v>
       </c>
     </row>
@@ -4372,16 +4390,16 @@
       <c r="A47" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="1">
         <v>550</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4389,16 +4407,16 @@
       <c r="A48" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="1">
         <v>729</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4406,16 +4424,16 @@
       <c r="A49" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="1">
         <v>560</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4423,16 +4441,16 @@
       <c r="A50" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="1">
         <v>375</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4440,16 +4458,16 @@
       <c r="A51" t="s">
         <v>38</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="1">
         <v>650</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4457,7 +4475,7 @@
       <c r="A52" t="s">
         <v>38</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C52" t="s">
@@ -4466,7 +4484,7 @@
       <c r="D52">
         <v>1118</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="9">
         <v>1</v>
       </c>
     </row>
@@ -4474,16 +4492,16 @@
       <c r="A53" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D53">
         <v>650</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="9">
         <v>1</v>
       </c>
     </row>
@@ -4491,16 +4509,16 @@
       <c r="A54" t="s">
         <v>38</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D54">
         <v>1000</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="9">
         <v>1</v>
       </c>
     </row>
@@ -4508,21 +4526,21 @@
       <c r="A55" t="s">
         <v>38</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D55">
         <v>630</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>